<commit_message>
Update to CCtests Sheets
Updated to support the new column inversion
</commit_message>
<xml_diff>
--- a/tests/CoordinateCheckerTests/Sheets/TestSheet_util.xlsx
+++ b/tests/CoordinateCheckerTests/Sheets/TestSheet_util.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\PycharmProjects\Geolocation\Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\PycharmProjects\Geolocation\CoordinateCheckerTests\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,10 +630,10 @@
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="12">
+        <v>45.467039999999997</v>
+      </c>
+      <c r="J2" s="12">
         <v>8.8957999999999995</v>
-      </c>
-      <c r="J2" s="12">
-        <v>45.467039999999997</v>
       </c>
       <c r="K2" s="13"/>
     </row>
@@ -661,10 +661,10 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="12">
+        <v>45.467509999999997</v>
+      </c>
+      <c r="J3" s="12">
         <v>8.8872800000000005</v>
-      </c>
-      <c r="J3" s="12">
-        <v>45.467509999999997</v>
       </c>
       <c r="K3" s="13"/>
     </row>
@@ -692,10 +692,10 @@
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="12">
+        <v>45.465780000000002</v>
+      </c>
+      <c r="J4" s="12">
         <v>8.8602000000000007</v>
-      </c>
-      <c r="J4" s="12">
-        <v>45.465780000000002</v>
       </c>
       <c r="K4" s="13"/>
     </row>
@@ -706,6 +706,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010058DA66D638BE7B44B507062379ADF5A7" ma:contentTypeVersion="13" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8ae68a76cb13176a9bd3869cbbaba6a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0bbe7d74-8f18-4455-bcbe-03c409394a09" xmlns:ns4="3652809a-078f-4ce1-86ee-e4a946add5f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f18eac86622072384597db78bf044af" ns3:_="" ns4:_="">
     <xsd:import namespace="0bbe7d74-8f18-4455-bcbe-03c409394a09"/>
@@ -928,15 +937,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -944,6 +944,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D17A7BC-6F05-4765-9458-B459D27A64E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3D50F8A-4330-4E5C-9A23-836DB50B14F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -962,14 +970,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D17A7BC-6F05-4765-9458-B459D27A64E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81CCD08-275C-47A2-9EEC-2E10E438FB52}">
   <ds:schemaRefs>

</xml_diff>